<commit_message>
update Reclaimer country-specific with minor structure change
</commit_message>
<xml_diff>
--- a/exposan/biogenic_refinery/results/sysA_Uganda.xlsx
+++ b/exposan/biogenic_refinery/results/sysA_Uganda.xlsx
@@ -15163,7 +15163,7 @@
         <v>67.35540000000003</v>
       </c>
       <c r="E11">
-        <v>5.688094650588658</v>
+        <v>5.688094650588657</v>
       </c>
       <c r="F11">
         <v>41.44787167912876</v>
@@ -25180,7 +25180,7 @@
         <v>67.35540000000003</v>
       </c>
       <c r="E7">
-        <v>5.954616018349608</v>
+        <v>5.954616018349607</v>
       </c>
       <c r="F7">
         <v>34.6186697216243</v>
@@ -44639,7 +44639,7 @@
         <v>67.35540000000003</v>
       </c>
       <c r="OA11">
-        <v>5.688094650588658</v>
+        <v>5.688094650588657</v>
       </c>
       <c r="OB11">
         <v>41.44787167912876</v>

</xml_diff>